<commit_message>
Initial commit: Flask e-commerce app
</commit_message>
<xml_diff>
--- a/data_new.xlsx
+++ b/data_new.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Users" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Products" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Orders" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Users" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Products" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Orders" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,6 +459,56 @@
       <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Role</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>vinit</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>scrypt:32768:8:1$3YqEzykj0MTLFiSJ$5320671aedef4422c96ec1a1dcb161a5f997c13be9e432d6a8e39e2e5743698b4b3673d4ea5777ebb26f04c063d19152e252cc55986a070f23e396c173f26958</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>vinit.j6666@gmail.com</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Seller</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>vinit.jadhav</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>scrypt:32768:8:1$bcv8YdL86dxDloMF$e659e065445662d7f7a0c59e46c6b32f3244be4bc9a47a25c73073f1701a7a47efc173ecc0e16206424cce9ad5d53b379cba51aaa6c3492f1bdeecdd2d20c166</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>vinit.jadhav.vj123@gmail.com</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Seller</t>
         </is>
       </c>
     </row>

</xml_diff>